<commit_message>
dantq phan lại folder
</commit_message>
<xml_diff>
--- a/Analysis/Application_Of_Trademark.xlsx
+++ b/Analysis/Application_Of_Trademark.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5528EB-544F-451E-8B67-BFC4442C3CAA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3172808F-A896-4B76-8028-4CF0C14CAD38}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,15 +631,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
     <col min="5" max="5" width="39.7109375" customWidth="1"/>
     <col min="6" max="6" width="55.28515625" customWidth="1"/>
   </cols>

</xml_diff>